<commit_message>
Add another example file, add STR ingress function
</commit_message>
<xml_diff>
--- a/ExampleSTR.xlsx
+++ b/ExampleSTR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jandrews\Documents\GitHub\strprofiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC3C251A-1028-4473-98F1-CA08AFA221E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EEB3A5D-254B-4DC9-A4E1-F6E5FC76D62D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1286,7 +1286,7 @@
   <dimension ref="A1:DG73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="O48" sqref="O48"/>
+      <selection activeCell="Q47" sqref="Q47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17726,7 +17726,7 @@
         <v>9040</v>
       </c>
       <c r="F50">
-        <v>17.3</v>
+        <v>16.3</v>
       </c>
       <c r="G50">
         <v>195.28</v>
@@ -20070,15 +20070,6 @@
       <c r="E57">
         <v>7595</v>
       </c>
-      <c r="F57">
-        <v>10</v>
-      </c>
-      <c r="G57">
-        <v>420.11</v>
-      </c>
-      <c r="H57">
-        <v>9040</v>
-      </c>
       <c r="I57" t="s">
         <v>110</v>
       </c>
@@ -21076,7 +21067,7 @@
         <v>10513</v>
       </c>
       <c r="F60">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G60">
         <v>300.58999999999997</v>

</xml_diff>

<commit_message>
Fix sample ingress, add scoring function
</commit_message>
<xml_diff>
--- a/ExampleSTR.xlsx
+++ b/ExampleSTR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jandrews\Documents\GitHub\strprofiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EEB3A5D-254B-4DC9-A4E1-F6E5FC76D62D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA04AB32-D27E-40B2-8AC7-0AD88754D00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7840" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7976" uniqueCount="141">
   <si>
     <t xml:space="preserve"> Sample Name</t>
   </si>
@@ -441,6 +441,9 @@
   </si>
   <si>
     <t>Sample3</t>
+  </si>
+  <si>
+    <t>Sample11</t>
   </si>
 </sst>
 </file>
@@ -1283,10 +1286,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DG73"/>
+  <dimension ref="A1:DG95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="Q47" sqref="Q47"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="N78" sqref="N78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2324,8 +2327,8 @@
       <c r="H4">
         <v>5467</v>
       </c>
-      <c r="I4" t="s">
-        <v>110</v>
+      <c r="I4">
+        <v>16</v>
       </c>
       <c r="J4" t="s">
         <v>110</v>
@@ -25740,9 +25743,779 @@
         <v>110</v>
       </c>
     </row>
+    <row r="74" spans="1:111" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>140</v>
+      </c>
+      <c r="B74" t="s">
+        <v>114</v>
+      </c>
+      <c r="C74">
+        <v>12</v>
+      </c>
+      <c r="D74">
+        <v>172.08</v>
+      </c>
+      <c r="E74">
+        <v>9240</v>
+      </c>
+      <c r="F74">
+        <v>17.3</v>
+      </c>
+      <c r="G74">
+        <v>195.29</v>
+      </c>
+      <c r="H74">
+        <v>4453</v>
+      </c>
+      <c r="I74">
+        <v>18.3</v>
+      </c>
+      <c r="J74">
+        <v>199.28</v>
+      </c>
+      <c r="K74">
+        <v>4393</v>
+      </c>
+    </row>
+    <row r="75" spans="1:111" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>140</v>
+      </c>
+      <c r="B75" t="s">
+        <v>122</v>
+      </c>
+      <c r="C75" t="s">
+        <v>110</v>
+      </c>
+      <c r="D75" t="s">
+        <v>110</v>
+      </c>
+      <c r="E75" t="s">
+        <v>110</v>
+      </c>
+      <c r="F75" t="s">
+        <v>110</v>
+      </c>
+      <c r="G75" t="s">
+        <v>110</v>
+      </c>
+      <c r="H75" t="s">
+        <v>110</v>
+      </c>
+      <c r="I75" t="s">
+        <v>110</v>
+      </c>
+      <c r="J75" t="s">
+        <v>110</v>
+      </c>
+      <c r="K75" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="76" spans="1:111" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>140</v>
+      </c>
+      <c r="B76" t="s">
+        <v>128</v>
+      </c>
+      <c r="C76">
+        <v>16</v>
+      </c>
+      <c r="D76">
+        <v>128.29</v>
+      </c>
+      <c r="E76">
+        <v>8268</v>
+      </c>
+      <c r="F76">
+        <v>18</v>
+      </c>
+      <c r="G76">
+        <v>136.84</v>
+      </c>
+      <c r="H76">
+        <v>5467</v>
+      </c>
+      <c r="I76">
+        <v>16</v>
+      </c>
+      <c r="J76" t="s">
+        <v>110</v>
+      </c>
+      <c r="K76" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="77" spans="1:111" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>140</v>
+      </c>
+      <c r="B77" t="s">
+        <v>125</v>
+      </c>
+      <c r="C77">
+        <v>12</v>
+      </c>
+      <c r="D77">
+        <v>110.7</v>
+      </c>
+      <c r="E77">
+        <v>9660</v>
+      </c>
+      <c r="F77">
+        <v>13</v>
+      </c>
+      <c r="G77">
+        <v>115.17</v>
+      </c>
+      <c r="H77">
+        <v>5215</v>
+      </c>
+      <c r="I77" t="s">
+        <v>110</v>
+      </c>
+      <c r="J77" t="s">
+        <v>110</v>
+      </c>
+      <c r="K77" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="78" spans="1:111" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>140</v>
+      </c>
+      <c r="B78" t="s">
+        <v>131</v>
+      </c>
+      <c r="C78">
+        <v>9</v>
+      </c>
+      <c r="D78">
+        <v>415.04</v>
+      </c>
+      <c r="E78">
+        <v>5099</v>
+      </c>
+      <c r="F78">
+        <v>13</v>
+      </c>
+      <c r="G78">
+        <v>435.88</v>
+      </c>
+      <c r="H78">
+        <v>9426</v>
+      </c>
+      <c r="I78" t="s">
+        <v>110</v>
+      </c>
+      <c r="J78" t="s">
+        <v>110</v>
+      </c>
+      <c r="K78" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="79" spans="1:111" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>140</v>
+      </c>
+      <c r="B79" t="s">
+        <v>112</v>
+      </c>
+      <c r="C79">
+        <v>11</v>
+      </c>
+      <c r="D79">
+        <v>344.75</v>
+      </c>
+      <c r="E79">
+        <v>13691</v>
+      </c>
+      <c r="F79">
+        <v>12</v>
+      </c>
+      <c r="G79">
+        <v>348.69</v>
+      </c>
+      <c r="H79">
+        <v>8923</v>
+      </c>
+      <c r="I79" t="s">
+        <v>110</v>
+      </c>
+      <c r="J79" t="s">
+        <v>110</v>
+      </c>
+      <c r="K79" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="80" spans="1:111" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>140</v>
+      </c>
+      <c r="B80" t="s">
+        <v>133</v>
+      </c>
+      <c r="C80">
+        <v>10</v>
+      </c>
+      <c r="D80">
+        <v>87.41</v>
+      </c>
+      <c r="E80">
+        <v>18671</v>
+      </c>
+      <c r="F80">
+        <v>15</v>
+      </c>
+      <c r="G80">
+        <v>109.89</v>
+      </c>
+      <c r="H80">
+        <v>9667</v>
+      </c>
+      <c r="I80" t="s">
+        <v>110</v>
+      </c>
+      <c r="J80" t="s">
+        <v>110</v>
+      </c>
+      <c r="K80" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>140</v>
+      </c>
+      <c r="B81" t="s">
+        <v>113</v>
+      </c>
+      <c r="C81">
+        <v>15</v>
+      </c>
+      <c r="D81">
+        <v>455.95</v>
+      </c>
+      <c r="E81">
+        <v>13504</v>
+      </c>
+      <c r="F81">
+        <v>17</v>
+      </c>
+      <c r="G81">
+        <v>462.06</v>
+      </c>
+      <c r="H81">
+        <v>6186</v>
+      </c>
+      <c r="I81" t="s">
+        <v>110</v>
+      </c>
+      <c r="J81" t="s">
+        <v>110</v>
+      </c>
+      <c r="K81" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>140</v>
+      </c>
+      <c r="B82" t="s">
+        <v>117</v>
+      </c>
+      <c r="C82">
+        <v>12</v>
+      </c>
+      <c r="D82">
+        <v>153.72</v>
+      </c>
+      <c r="E82">
+        <v>9134</v>
+      </c>
+      <c r="F82">
+        <v>16</v>
+      </c>
+      <c r="G82">
+        <v>170.48</v>
+      </c>
+      <c r="H82">
+        <v>10501</v>
+      </c>
+      <c r="I82" t="s">
+        <v>110</v>
+      </c>
+      <c r="J82" t="s">
+        <v>110</v>
+      </c>
+      <c r="K82" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>140</v>
+      </c>
+      <c r="B83" t="s">
+        <v>118</v>
+      </c>
+      <c r="C83">
+        <v>20</v>
+      </c>
+      <c r="D83">
+        <v>263.91000000000003</v>
+      </c>
+      <c r="E83">
+        <v>3209</v>
+      </c>
+      <c r="F83">
+        <v>22</v>
+      </c>
+      <c r="G83">
+        <v>267.97000000000003</v>
+      </c>
+      <c r="H83">
+        <v>3834</v>
+      </c>
+      <c r="I83" t="s">
+        <v>110</v>
+      </c>
+      <c r="J83" t="s">
+        <v>110</v>
+      </c>
+      <c r="K83" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>140</v>
+      </c>
+      <c r="B84" t="s">
+        <v>126</v>
+      </c>
+      <c r="C84">
+        <v>7</v>
+      </c>
+      <c r="D84">
+        <v>85.33</v>
+      </c>
+      <c r="E84">
+        <v>8305</v>
+      </c>
+      <c r="F84">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="G84">
+        <v>97.43</v>
+      </c>
+      <c r="H84">
+        <v>7853</v>
+      </c>
+      <c r="I84" t="s">
+        <v>110</v>
+      </c>
+      <c r="J84" t="s">
+        <v>110</v>
+      </c>
+      <c r="K84" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>140</v>
+      </c>
+      <c r="B85" t="s">
+        <v>111</v>
+      </c>
+      <c r="C85">
+        <v>14</v>
+      </c>
+      <c r="D85">
+        <v>144.47</v>
+      </c>
+      <c r="E85">
+        <v>7151</v>
+      </c>
+      <c r="F85">
+        <v>16</v>
+      </c>
+      <c r="G85">
+        <v>148.53</v>
+      </c>
+      <c r="H85">
+        <v>8447</v>
+      </c>
+      <c r="I85" t="s">
+        <v>110</v>
+      </c>
+      <c r="J85" t="s">
+        <v>110</v>
+      </c>
+      <c r="K85" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>140</v>
+      </c>
+      <c r="B86" t="s">
+        <v>120</v>
+      </c>
+      <c r="C86">
+        <v>10</v>
+      </c>
+      <c r="D86">
+        <v>292.51</v>
+      </c>
+      <c r="E86">
+        <v>12340</v>
+      </c>
+      <c r="F86">
+        <v>14</v>
+      </c>
+      <c r="G86">
+        <v>308.70999999999998</v>
+      </c>
+      <c r="H86">
+        <v>11784</v>
+      </c>
+      <c r="I86" t="s">
+        <v>110</v>
+      </c>
+      <c r="J86" t="s">
+        <v>110</v>
+      </c>
+      <c r="K86" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>140</v>
+      </c>
+      <c r="B87" t="s">
+        <v>121</v>
+      </c>
+      <c r="C87">
+        <v>15</v>
+      </c>
+      <c r="D87">
+        <v>141.53</v>
+      </c>
+      <c r="E87">
+        <v>12870</v>
+      </c>
+      <c r="F87">
+        <v>18.3</v>
+      </c>
+      <c r="G87">
+        <v>157.12</v>
+      </c>
+      <c r="H87">
+        <v>13731</v>
+      </c>
+      <c r="I87" t="s">
+        <v>110</v>
+      </c>
+      <c r="J87" t="s">
+        <v>110</v>
+      </c>
+      <c r="K87" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>140</v>
+      </c>
+      <c r="B88" t="s">
+        <v>134</v>
+      </c>
+      <c r="C88" t="s">
+        <v>135</v>
+      </c>
+      <c r="D88">
+        <v>81.97</v>
+      </c>
+      <c r="E88">
+        <v>16696</v>
+      </c>
+      <c r="F88" t="s">
+        <v>110</v>
+      </c>
+      <c r="G88" t="s">
+        <v>110</v>
+      </c>
+      <c r="H88" t="s">
+        <v>110</v>
+      </c>
+      <c r="I88" t="s">
+        <v>110</v>
+      </c>
+      <c r="J88" t="s">
+        <v>110</v>
+      </c>
+      <c r="K88" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>140</v>
+      </c>
+      <c r="B89" t="s">
+        <v>115</v>
+      </c>
+      <c r="C89">
+        <v>16</v>
+      </c>
+      <c r="D89">
+        <v>283.82</v>
+      </c>
+      <c r="E89">
+        <v>8469</v>
+      </c>
+      <c r="F89" t="s">
+        <v>110</v>
+      </c>
+      <c r="G89" t="s">
+        <v>110</v>
+      </c>
+      <c r="H89" t="s">
+        <v>110</v>
+      </c>
+      <c r="I89" t="s">
+        <v>110</v>
+      </c>
+      <c r="J89" t="s">
+        <v>110</v>
+      </c>
+      <c r="K89" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>140</v>
+      </c>
+      <c r="B90" t="s">
+        <v>116</v>
+      </c>
+      <c r="C90">
+        <v>12</v>
+      </c>
+      <c r="D90">
+        <v>328.21</v>
+      </c>
+      <c r="E90">
+        <v>7079</v>
+      </c>
+      <c r="F90" t="s">
+        <v>110</v>
+      </c>
+      <c r="G90" t="s">
+        <v>110</v>
+      </c>
+      <c r="H90" t="s">
+        <v>110</v>
+      </c>
+      <c r="I90" t="s">
+        <v>110</v>
+      </c>
+      <c r="J90" t="s">
+        <v>110</v>
+      </c>
+      <c r="K90" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>140</v>
+      </c>
+      <c r="B91" t="s">
+        <v>129</v>
+      </c>
+      <c r="C91">
+        <v>12</v>
+      </c>
+      <c r="D91">
+        <v>345.11</v>
+      </c>
+      <c r="E91">
+        <v>14598</v>
+      </c>
+      <c r="F91" t="s">
+        <v>110</v>
+      </c>
+      <c r="G91" t="s">
+        <v>110</v>
+      </c>
+      <c r="H91" t="s">
+        <v>110</v>
+      </c>
+      <c r="I91" t="s">
+        <v>110</v>
+      </c>
+      <c r="J91" t="s">
+        <v>110</v>
+      </c>
+      <c r="K91" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>140</v>
+      </c>
+      <c r="B92" t="s">
+        <v>119</v>
+      </c>
+      <c r="C92">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="D92">
+        <v>239.67</v>
+      </c>
+      <c r="E92">
+        <v>19231</v>
+      </c>
+      <c r="F92" t="s">
+        <v>110</v>
+      </c>
+      <c r="G92" t="s">
+        <v>110</v>
+      </c>
+      <c r="H92" t="s">
+        <v>110</v>
+      </c>
+      <c r="I92" t="s">
+        <v>110</v>
+      </c>
+      <c r="J92" t="s">
+        <v>110</v>
+      </c>
+      <c r="K92" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>140</v>
+      </c>
+      <c r="B93" t="s">
+        <v>132</v>
+      </c>
+      <c r="C93">
+        <v>11</v>
+      </c>
+      <c r="D93">
+        <v>424.02</v>
+      </c>
+      <c r="E93">
+        <v>12239</v>
+      </c>
+      <c r="F93" t="s">
+        <v>110</v>
+      </c>
+      <c r="G93" t="s">
+        <v>110</v>
+      </c>
+      <c r="H93" t="s">
+        <v>110</v>
+      </c>
+      <c r="I93" t="s">
+        <v>110</v>
+      </c>
+      <c r="J93" t="s">
+        <v>110</v>
+      </c>
+      <c r="K93" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>140</v>
+      </c>
+      <c r="B94" t="s">
+        <v>127</v>
+      </c>
+      <c r="C94">
+        <v>14</v>
+      </c>
+      <c r="D94">
+        <v>228.37</v>
+      </c>
+      <c r="E94">
+        <v>14273</v>
+      </c>
+      <c r="F94" t="s">
+        <v>110</v>
+      </c>
+      <c r="G94" t="s">
+        <v>110</v>
+      </c>
+      <c r="H94" t="s">
+        <v>110</v>
+      </c>
+      <c r="I94" t="s">
+        <v>110</v>
+      </c>
+      <c r="J94" t="s">
+        <v>110</v>
+      </c>
+      <c r="K94" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>140</v>
+      </c>
+      <c r="B95" t="s">
+        <v>130</v>
+      </c>
+      <c r="C95">
+        <v>23</v>
+      </c>
+      <c r="D95">
+        <v>302.23</v>
+      </c>
+      <c r="E95">
+        <v>14599</v>
+      </c>
+      <c r="F95" t="s">
+        <v>110</v>
+      </c>
+      <c r="G95" t="s">
+        <v>110</v>
+      </c>
+      <c r="H95" t="s">
+        <v>110</v>
+      </c>
+      <c r="I95" t="s">
+        <v>110</v>
+      </c>
+      <c r="J95" t="s">
+        <v>110</v>
+      </c>
+      <c r="K95" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:DG1201">
-    <sortCondition ref="A2:A1201"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:DG1199">
+    <sortCondition ref="A2:A1199"/>
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add penta_fix, mixing check, program logic.
Functional version.
</commit_message>
<xml_diff>
--- a/ExampleSTR.xlsx
+++ b/ExampleSTR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jandrews\Documents\GitHub\strprofiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA04AB32-D27E-40B2-8AC7-0AD88754D00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F692BE77-E733-4F78-BDAA-276B4F66AA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GMK582 Zhang Genotypes Table" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7976" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7970" uniqueCount="141">
   <si>
     <t xml:space="preserve"> Sample Name</t>
   </si>
@@ -1288,8 +1288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DG95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="N78" sqref="N78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11372,8 +11372,8 @@
       <c r="H31">
         <v>10160</v>
       </c>
-      <c r="I31" t="s">
-        <v>110</v>
+      <c r="I31">
+        <v>19</v>
       </c>
       <c r="J31" t="s">
         <v>110</v>
@@ -12042,8 +12042,8 @@
       <c r="H33">
         <v>8497</v>
       </c>
-      <c r="I33" t="s">
-        <v>110</v>
+      <c r="I33">
+        <v>18</v>
       </c>
       <c r="J33" t="s">
         <v>110</v>
@@ -12377,8 +12377,8 @@
       <c r="H34">
         <v>9182</v>
       </c>
-      <c r="I34" t="s">
-        <v>110</v>
+      <c r="I34">
+        <v>19</v>
       </c>
       <c r="J34" t="s">
         <v>110</v>
@@ -12712,8 +12712,8 @@
       <c r="H35">
         <v>3863</v>
       </c>
-      <c r="I35" t="s">
-        <v>110</v>
+      <c r="I35">
+        <v>29</v>
       </c>
       <c r="J35" t="s">
         <v>110</v>
@@ -13047,8 +13047,8 @@
       <c r="H36">
         <v>10472</v>
       </c>
-      <c r="I36" t="s">
-        <v>110</v>
+      <c r="I36">
+        <v>16</v>
       </c>
       <c r="J36" t="s">
         <v>110</v>
@@ -13382,8 +13382,8 @@
       <c r="H37">
         <v>7945</v>
       </c>
-      <c r="I37" t="s">
-        <v>110</v>
+      <c r="I37">
+        <v>12</v>
       </c>
       <c r="J37" t="s">
         <v>110</v>

</xml_diff>

<commit_message>
Remove duplicate alleles from output.
</commit_message>
<xml_diff>
--- a/ExampleSTR.xlsx
+++ b/ExampleSTR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jandrews\Documents\GitHub\strprofiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F692BE77-E733-4F78-BDAA-276B4F66AA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D01DA52-DA69-4558-95D5-C1DEB5F7F23E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GMK582 Zhang Genotypes Table" sheetId="1" r:id="rId1"/>
@@ -1289,7 +1289,7 @@
   <dimension ref="A1:DG95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>